<commit_message>
Atualização de bases das ligas, do dia: 18-05-2024 às 14:13
</commit_message>
<xml_diff>
--- a/Bosnia Herzegovina Premier Liga/Bosnia Herzegovina Premier Liga.xlsx
+++ b/Bosnia Herzegovina Premier Liga/Bosnia Herzegovina Premier Liga.xlsx
@@ -1206,7 +1206,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6865285</v>
+        <v>6865281</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1215,13 +1215,13 @@
         <v>45150.5</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1230,19 +1230,19 @@
         <v>42</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="K9">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="L9">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="M9">
-        <v>1.909</v>
+        <v>1.75</v>
       </c>
       <c r="N9">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="O9">
         <v>3.4</v>
@@ -1251,10 +1251,10 @@
         <v>-0.5</v>
       </c>
       <c r="Q9">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="R9">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="S9">
         <v>2.5</v>
@@ -1266,7 +1266,7 @@
         <v>1.95</v>
       </c>
       <c r="V9">
-        <v>0.909</v>
+        <v>0.75</v>
       </c>
       <c r="W9">
         <v>-1</v>
@@ -1275,7 +1275,7 @@
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="Z9">
         <v>-1</v>
@@ -1292,7 +1292,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6865281</v>
+        <v>6865285</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1301,13 +1301,13 @@
         <v>45150.5</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1316,19 +1316,19 @@
         <v>42</v>
       </c>
       <c r="J10">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="L10">
+        <v>3.2</v>
+      </c>
+      <c r="M10">
+        <v>1.909</v>
+      </c>
+      <c r="N10">
         <v>3.5</v>
-      </c>
-      <c r="M10">
-        <v>1.75</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
       </c>
       <c r="O10">
         <v>3.4</v>
@@ -1337,10 +1337,10 @@
         <v>-0.5</v>
       </c>
       <c r="Q10">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="R10">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="S10">
         <v>2.5</v>
@@ -1352,7 +1352,7 @@
         <v>1.95</v>
       </c>
       <c r="V10">
-        <v>0.75</v>
+        <v>0.909</v>
       </c>
       <c r="W10">
         <v>-1</v>
@@ -1361,7 +1361,7 @@
         <v>-1</v>
       </c>
       <c r="Y10">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="Z10">
         <v>-1</v>
@@ -3528,7 +3528,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6864629</v>
+        <v>6865299</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
@@ -3537,58 +3537,58 @@
         <v>45186.61458333334</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
         <v>1</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>42</v>
       </c>
       <c r="J36">
-        <v>1.363</v>
+        <v>1.25</v>
       </c>
       <c r="K36">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="L36">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="M36">
-        <v>1.363</v>
+        <v>1.4</v>
       </c>
       <c r="N36">
-        <v>4.2</v>
+        <v>4.75</v>
       </c>
       <c r="O36">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="P36">
         <v>-1.25</v>
       </c>
       <c r="Q36">
+        <v>1.9</v>
+      </c>
+      <c r="R36">
+        <v>1.9</v>
+      </c>
+      <c r="S36">
+        <v>2.75</v>
+      </c>
+      <c r="T36">
+        <v>1.85</v>
+      </c>
+      <c r="U36">
         <v>1.95</v>
       </c>
-      <c r="R36">
-        <v>1.85</v>
-      </c>
-      <c r="S36">
-        <v>2.5</v>
-      </c>
-      <c r="T36">
-        <v>1.925</v>
-      </c>
-      <c r="U36">
-        <v>1.875</v>
-      </c>
       <c r="V36">
-        <v>0.363</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W36">
         <v>-1</v>
@@ -3600,13 +3600,13 @@
         <v>-0.5</v>
       </c>
       <c r="Z36">
+        <v>0.45</v>
+      </c>
+      <c r="AA36">
         <v>0.425</v>
       </c>
-      <c r="AA36">
-        <v>-1</v>
-      </c>
       <c r="AB36">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -3614,7 +3614,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6865299</v>
+        <v>6864629</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
@@ -3623,58 +3623,58 @@
         <v>45186.61458333334</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>42</v>
       </c>
       <c r="J37">
-        <v>1.25</v>
+        <v>1.363</v>
       </c>
       <c r="K37">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="L37">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="M37">
-        <v>1.4</v>
+        <v>1.363</v>
       </c>
       <c r="N37">
-        <v>4.75</v>
+        <v>4.2</v>
       </c>
       <c r="O37">
-        <v>5.75</v>
+        <v>6.5</v>
       </c>
       <c r="P37">
         <v>-1.25</v>
       </c>
       <c r="Q37">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="R37">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="S37">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="T37">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="U37">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V37">
-        <v>0.3999999999999999</v>
+        <v>0.363</v>
       </c>
       <c r="W37">
         <v>-1</v>
@@ -3686,13 +3686,13 @@
         <v>-0.5</v>
       </c>
       <c r="Z37">
-        <v>0.45</v>
+        <v>0.425</v>
       </c>
       <c r="AA37">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AB37">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -4646,7 +4646,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6865311</v>
+        <v>6865310</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -4655,76 +4655,76 @@
         <v>45200.41666666666</v>
       </c>
       <c r="E49" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H49">
         <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J49">
-        <v>1.833</v>
+        <v>3.4</v>
       </c>
       <c r="K49">
         <v>3.6</v>
       </c>
       <c r="L49">
-        <v>3.4</v>
+        <v>1.833</v>
       </c>
       <c r="M49">
-        <v>1.909</v>
+        <v>4.75</v>
       </c>
       <c r="N49">
-        <v>3.4</v>
+        <v>4.75</v>
       </c>
       <c r="O49">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="P49">
-        <v>-0.5</v>
+        <v>1.25</v>
       </c>
       <c r="Q49">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="R49">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S49">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T49">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="U49">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V49">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="W49">
         <v>-1</v>
       </c>
       <c r="X49">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Y49">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="Z49">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA49">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB49">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="50" spans="1:28">
@@ -4732,7 +4732,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>6865310</v>
+        <v>6865311</v>
       </c>
       <c r="C50" t="s">
         <v>27</v>
@@ -4741,76 +4741,76 @@
         <v>45200.41666666666</v>
       </c>
       <c r="E50" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H50">
         <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J50">
-        <v>3.4</v>
+        <v>1.833</v>
       </c>
       <c r="K50">
         <v>3.6</v>
       </c>
       <c r="L50">
-        <v>1.833</v>
+        <v>3.4</v>
       </c>
       <c r="M50">
-        <v>4.75</v>
+        <v>1.909</v>
       </c>
       <c r="N50">
-        <v>4.75</v>
+        <v>3.4</v>
       </c>
       <c r="O50">
-        <v>1.45</v>
+        <v>3.3</v>
       </c>
       <c r="P50">
-        <v>1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q50">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="R50">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="S50">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T50">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U50">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V50">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="W50">
         <v>-1</v>
       </c>
       <c r="X50">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="Y50">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z50">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA50">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB50">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="51" spans="1:28">
@@ -6968,7 +6968,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>6865328</v>
+        <v>6865377</v>
       </c>
       <c r="C76" t="s">
         <v>27</v>
@@ -6977,76 +6977,76 @@
         <v>45235.375</v>
       </c>
       <c r="E76" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F76" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J76">
-        <v>2</v>
+        <v>1.333</v>
       </c>
       <c r="K76">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L76">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M76">
-        <v>2.1</v>
+        <v>1.166</v>
       </c>
       <c r="N76">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="O76">
-        <v>3.3</v>
+        <v>13</v>
       </c>
       <c r="P76">
-        <v>-0.25</v>
+        <v>-2</v>
       </c>
       <c r="Q76">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="R76">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S76">
-        <v>2</v>
+        <v>3.25</v>
       </c>
       <c r="T76">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U76">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V76">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="W76">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X76">
         <v>-1</v>
       </c>
       <c r="Y76">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Z76">
-        <v>0.4875</v>
+        <v>0</v>
       </c>
       <c r="AA76">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AB76">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="77" spans="1:28">
@@ -7054,7 +7054,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>6865377</v>
+        <v>6865328</v>
       </c>
       <c r="C77" t="s">
         <v>27</v>
@@ -7063,76 +7063,76 @@
         <v>45235.375</v>
       </c>
       <c r="E77" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F77" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J77">
-        <v>1.333</v>
+        <v>2</v>
       </c>
       <c r="K77">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L77">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M77">
-        <v>1.166</v>
+        <v>2.1</v>
       </c>
       <c r="N77">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="O77">
-        <v>13</v>
+        <v>3.3</v>
       </c>
       <c r="P77">
-        <v>-2</v>
+        <v>-0.25</v>
       </c>
       <c r="Q77">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="R77">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S77">
-        <v>3.25</v>
+        <v>2</v>
       </c>
       <c r="T77">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="U77">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V77">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W77">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X77">
         <v>-1</v>
       </c>
       <c r="Y77">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Z77">
-        <v>0</v>
+        <v>0.4875</v>
       </c>
       <c r="AA77">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AB77">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:28">
@@ -7914,7 +7914,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>7505497</v>
+        <v>7505495</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
@@ -7923,76 +7923,76 @@
         <v>45256.375</v>
       </c>
       <c r="E87" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F87" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J87">
-        <v>1.65</v>
+        <v>1.444</v>
       </c>
       <c r="K87">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="L87">
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="M87">
+        <v>1.5</v>
+      </c>
+      <c r="N87">
+        <v>4.2</v>
+      </c>
+      <c r="O87">
+        <v>5.25</v>
+      </c>
+      <c r="P87">
+        <v>-1</v>
+      </c>
+      <c r="Q87">
         <v>1.8</v>
       </c>
-      <c r="N87">
-        <v>3.2</v>
-      </c>
-      <c r="O87">
-        <v>4.2</v>
-      </c>
-      <c r="P87">
-        <v>-0.5</v>
-      </c>
-      <c r="Q87">
-        <v>1.825</v>
-      </c>
       <c r="R87">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S87">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="T87">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="U87">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="V87">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="W87">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="X87">
         <v>-1</v>
       </c>
       <c r="Y87">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z87">
-        <v>0.9750000000000001</v>
+        <v>0</v>
       </c>
       <c r="AA87">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB87">
-        <v>0</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="88" spans="1:28">
@@ -8000,7 +8000,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>7505495</v>
+        <v>7505497</v>
       </c>
       <c r="C88" t="s">
         <v>27</v>
@@ -8009,76 +8009,76 @@
         <v>45256.375</v>
       </c>
       <c r="E88" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G88">
         <v>1</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J88">
-        <v>1.444</v>
+        <v>1.65</v>
       </c>
       <c r="K88">
+        <v>3.4</v>
+      </c>
+      <c r="L88">
+        <v>4.75</v>
+      </c>
+      <c r="M88">
+        <v>1.8</v>
+      </c>
+      <c r="N88">
+        <v>3.2</v>
+      </c>
+      <c r="O88">
         <v>4.2</v>
       </c>
-      <c r="L88">
-        <v>5.5</v>
-      </c>
-      <c r="M88">
-        <v>1.5</v>
-      </c>
-      <c r="N88">
-        <v>4.2</v>
-      </c>
-      <c r="O88">
-        <v>5.25</v>
-      </c>
       <c r="P88">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Q88">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="R88">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S88">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="T88">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="U88">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="V88">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="W88">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="X88">
         <v>-1</v>
       </c>
       <c r="Y88">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z88">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA88">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB88">
-        <v>1.025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:28">
@@ -8946,7 +8946,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>6864639</v>
+        <v>6865343</v>
       </c>
       <c r="C99" t="s">
         <v>27</v>
@@ -8955,76 +8955,76 @@
         <v>45269.375</v>
       </c>
       <c r="E99" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F99" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G99">
         <v>1</v>
       </c>
       <c r="H99">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J99">
-        <v>11</v>
+        <v>1.909</v>
       </c>
       <c r="K99">
-        <v>6</v>
+        <v>3.3</v>
       </c>
       <c r="L99">
+        <v>3.5</v>
+      </c>
+      <c r="M99">
+        <v>2.2</v>
+      </c>
+      <c r="N99">
+        <v>2.8</v>
+      </c>
+      <c r="O99">
+        <v>3.3</v>
+      </c>
+      <c r="P99">
+        <v>-0.25</v>
+      </c>
+      <c r="Q99">
+        <v>1.95</v>
+      </c>
+      <c r="R99">
+        <v>1.85</v>
+      </c>
+      <c r="S99">
+        <v>1.75</v>
+      </c>
+      <c r="T99">
+        <v>1.875</v>
+      </c>
+      <c r="U99">
+        <v>1.925</v>
+      </c>
+      <c r="V99">
         <v>1.2</v>
       </c>
-      <c r="M99">
-        <v>10</v>
-      </c>
-      <c r="N99">
-        <v>6.5</v>
-      </c>
-      <c r="O99">
-        <v>1.181</v>
-      </c>
-      <c r="P99">
-        <v>2</v>
-      </c>
-      <c r="Q99">
-        <v>1.825</v>
-      </c>
-      <c r="R99">
-        <v>1.975</v>
-      </c>
-      <c r="S99">
-        <v>3</v>
-      </c>
-      <c r="T99">
-        <v>1.9</v>
-      </c>
-      <c r="U99">
-        <v>1.9</v>
-      </c>
-      <c r="V99">
-        <v>-1</v>
-      </c>
       <c r="W99">
         <v>-1</v>
       </c>
       <c r="X99">
-        <v>0.181</v>
+        <v>-1</v>
       </c>
       <c r="Y99">
-        <v>0.825</v>
+        <v>0.95</v>
       </c>
       <c r="Z99">
         <v>-1</v>
       </c>
       <c r="AA99">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB99">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="100" spans="1:28">
@@ -9032,7 +9032,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>6865343</v>
+        <v>6864639</v>
       </c>
       <c r="C100" t="s">
         <v>27</v>
@@ -9041,76 +9041,76 @@
         <v>45269.375</v>
       </c>
       <c r="E100" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F100" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G100">
         <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I100" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J100">
-        <v>1.909</v>
+        <v>11</v>
       </c>
       <c r="K100">
-        <v>3.3</v>
+        <v>6</v>
       </c>
       <c r="L100">
-        <v>3.5</v>
+        <v>1.2</v>
       </c>
       <c r="M100">
-        <v>2.2</v>
+        <v>10</v>
       </c>
       <c r="N100">
-        <v>2.8</v>
+        <v>6.5</v>
       </c>
       <c r="O100">
-        <v>3.3</v>
+        <v>1.181</v>
       </c>
       <c r="P100">
-        <v>-0.25</v>
+        <v>2</v>
       </c>
       <c r="Q100">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="R100">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S100">
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="T100">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="U100">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V100">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
       <c r="W100">
         <v>-1</v>
       </c>
       <c r="X100">
-        <v>-1</v>
+        <v>0.181</v>
       </c>
       <c r="Y100">
-        <v>0.95</v>
+        <v>0.825</v>
       </c>
       <c r="Z100">
         <v>-1</v>
       </c>
       <c r="AA100">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB100">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:28">
@@ -15654,7 +15654,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>7952769</v>
+        <v>7952767</v>
       </c>
       <c r="C177" t="s">
         <v>27</v>
@@ -15663,10 +15663,10 @@
         <v>45415.54166666666</v>
       </c>
       <c r="E177" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F177" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G177">
         <v>2</v>
@@ -15678,43 +15678,43 @@
         <v>42</v>
       </c>
       <c r="J177">
-        <v>1.666</v>
+        <v>1.727</v>
       </c>
       <c r="K177">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="L177">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="M177">
-        <v>1.333</v>
+        <v>1.3</v>
       </c>
       <c r="N177">
-        <v>4.2</v>
+        <v>4.333</v>
       </c>
       <c r="O177">
         <v>8</v>
       </c>
       <c r="P177">
-        <v>-1.25</v>
+        <v>-1.5</v>
       </c>
       <c r="Q177">
+        <v>1.95</v>
+      </c>
+      <c r="R177">
         <v>1.85</v>
       </c>
-      <c r="R177">
+      <c r="S177">
+        <v>2.75</v>
+      </c>
+      <c r="T177">
+        <v>1.85</v>
+      </c>
+      <c r="U177">
         <v>1.95</v>
       </c>
-      <c r="S177">
-        <v>2.25</v>
-      </c>
-      <c r="T177">
-        <v>1.9</v>
-      </c>
-      <c r="U177">
-        <v>1.9</v>
-      </c>
       <c r="V177">
-        <v>0.333</v>
+        <v>0.3</v>
       </c>
       <c r="W177">
         <v>-1</v>
@@ -15723,16 +15723,16 @@
         <v>-1</v>
       </c>
       <c r="Y177">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="Z177">
         <v>-1</v>
       </c>
       <c r="AA177">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB177">
-        <v>0.45</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="178" spans="1:28">
@@ -15740,7 +15740,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>7952767</v>
+        <v>7952769</v>
       </c>
       <c r="C178" t="s">
         <v>27</v>
@@ -15749,10 +15749,10 @@
         <v>45415.54166666666</v>
       </c>
       <c r="E178" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F178" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G178">
         <v>2</v>
@@ -15764,43 +15764,43 @@
         <v>42</v>
       </c>
       <c r="J178">
-        <v>1.727</v>
+        <v>1.666</v>
       </c>
       <c r="K178">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="L178">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="M178">
-        <v>1.3</v>
+        <v>1.333</v>
       </c>
       <c r="N178">
-        <v>4.333</v>
+        <v>4.2</v>
       </c>
       <c r="O178">
         <v>8</v>
       </c>
       <c r="P178">
-        <v>-1.5</v>
+        <v>-1.25</v>
       </c>
       <c r="Q178">
+        <v>1.85</v>
+      </c>
+      <c r="R178">
         <v>1.95</v>
       </c>
-      <c r="R178">
-        <v>1.85</v>
-      </c>
       <c r="S178">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T178">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="U178">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="V178">
-        <v>0.3</v>
+        <v>0.333</v>
       </c>
       <c r="W178">
         <v>-1</v>
@@ -15809,16 +15809,16 @@
         <v>-1</v>
       </c>
       <c r="Y178">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z178">
         <v>-1</v>
       </c>
       <c r="AA178">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB178">
-        <v>0.95</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="179" spans="1:28">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 22-05-2024 às 12:12
</commit_message>
<xml_diff>
--- a/Bosnia Herzegovina Premier Liga/Bosnia Herzegovina Premier Liga.xlsx
+++ b/Bosnia Herzegovina Premier Liga/Bosnia Herzegovina Premier Liga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -510,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB188"/>
+  <dimension ref="A1:AB194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1206,7 +1206,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6865281</v>
+        <v>6865285</v>
       </c>
       <c r="C9" t="s">
         <v>27</v>
@@ -1215,13 +1215,13 @@
         <v>45150.5</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1230,19 +1230,19 @@
         <v>42</v>
       </c>
       <c r="J9">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="L9">
+        <v>3.2</v>
+      </c>
+      <c r="M9">
+        <v>1.909</v>
+      </c>
+      <c r="N9">
         <v>3.5</v>
-      </c>
-      <c r="M9">
-        <v>1.75</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
       </c>
       <c r="O9">
         <v>3.4</v>
@@ -1251,10 +1251,10 @@
         <v>-0.5</v>
       </c>
       <c r="Q9">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="R9">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="S9">
         <v>2.5</v>
@@ -1266,7 +1266,7 @@
         <v>1.95</v>
       </c>
       <c r="V9">
-        <v>0.75</v>
+        <v>0.909</v>
       </c>
       <c r="W9">
         <v>-1</v>
@@ -1275,7 +1275,7 @@
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="Z9">
         <v>-1</v>
@@ -1292,7 +1292,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6865285</v>
+        <v>6865281</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -1301,13 +1301,13 @@
         <v>45150.5</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1316,19 +1316,19 @@
         <v>42</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="K10">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="L10">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="M10">
-        <v>1.909</v>
+        <v>1.75</v>
       </c>
       <c r="N10">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="O10">
         <v>3.4</v>
@@ -1337,10 +1337,10 @@
         <v>-0.5</v>
       </c>
       <c r="Q10">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="R10">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="S10">
         <v>2.5</v>
@@ -1352,7 +1352,7 @@
         <v>1.95</v>
       </c>
       <c r="V10">
-        <v>0.909</v>
+        <v>0.75</v>
       </c>
       <c r="W10">
         <v>-1</v>
@@ -1361,7 +1361,7 @@
         <v>-1</v>
       </c>
       <c r="Y10">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="Z10">
         <v>-1</v>
@@ -2926,7 +2926,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>6865296</v>
+        <v>6865295</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
@@ -2935,58 +2935,58 @@
         <v>45172.61458333334</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
         <v>1</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
       </c>
       <c r="I29" t="s">
         <v>42</v>
       </c>
       <c r="J29">
-        <v>1.909</v>
+        <v>1.8</v>
       </c>
       <c r="K29">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L29">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="M29">
+        <v>1.615</v>
+      </c>
+      <c r="N29">
+        <v>3.5</v>
+      </c>
+      <c r="O29">
+        <v>4.5</v>
+      </c>
+      <c r="P29">
+        <v>-0.75</v>
+      </c>
+      <c r="Q29">
+        <v>1.85</v>
+      </c>
+      <c r="R29">
         <v>1.95</v>
       </c>
-      <c r="N29">
-        <v>3.2</v>
-      </c>
-      <c r="O29">
-        <v>3.4</v>
-      </c>
-      <c r="P29">
-        <v>-0.5</v>
-      </c>
-      <c r="Q29">
-        <v>2.025</v>
-      </c>
-      <c r="R29">
-        <v>1.775</v>
-      </c>
       <c r="S29">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T29">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U29">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V29">
-        <v>0.95</v>
+        <v>0.615</v>
       </c>
       <c r="W29">
         <v>-1</v>
@@ -2995,16 +2995,16 @@
         <v>-1</v>
       </c>
       <c r="Y29">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z29">
         <v>-1</v>
       </c>
       <c r="AA29">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB29">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30" spans="1:28">
@@ -3012,7 +3012,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>6865295</v>
+        <v>6865296</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
@@ -3021,58 +3021,58 @@
         <v>45172.61458333334</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>42</v>
       </c>
       <c r="J30">
-        <v>1.8</v>
+        <v>1.909</v>
       </c>
       <c r="K30">
+        <v>3.2</v>
+      </c>
+      <c r="L30">
+        <v>3.6</v>
+      </c>
+      <c r="M30">
+        <v>1.95</v>
+      </c>
+      <c r="N30">
+        <v>3.2</v>
+      </c>
+      <c r="O30">
         <v>3.4</v>
       </c>
-      <c r="L30">
-        <v>3.8</v>
-      </c>
-      <c r="M30">
-        <v>1.615</v>
-      </c>
-      <c r="N30">
-        <v>3.5</v>
-      </c>
-      <c r="O30">
-        <v>4.5</v>
-      </c>
       <c r="P30">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q30">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="R30">
-        <v>1.95</v>
+        <v>1.775</v>
       </c>
       <c r="S30">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T30">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="U30">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V30">
-        <v>0.615</v>
+        <v>0.95</v>
       </c>
       <c r="W30">
         <v>-1</v>
@@ -3081,16 +3081,16 @@
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="Z30">
         <v>-1</v>
       </c>
       <c r="AA30">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB30">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:28">
@@ -3528,7 +3528,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6865299</v>
+        <v>6864629</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
@@ -3537,58 +3537,58 @@
         <v>45186.61458333334</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>42</v>
       </c>
       <c r="J36">
-        <v>1.25</v>
+        <v>1.363</v>
       </c>
       <c r="K36">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="L36">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="M36">
-        <v>1.4</v>
+        <v>1.363</v>
       </c>
       <c r="N36">
-        <v>4.75</v>
+        <v>4.2</v>
       </c>
       <c r="O36">
-        <v>5.75</v>
+        <v>6.5</v>
       </c>
       <c r="P36">
         <v>-1.25</v>
       </c>
       <c r="Q36">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="R36">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="S36">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="T36">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="U36">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V36">
-        <v>0.3999999999999999</v>
+        <v>0.363</v>
       </c>
       <c r="W36">
         <v>-1</v>
@@ -3600,13 +3600,13 @@
         <v>-0.5</v>
       </c>
       <c r="Z36">
-        <v>0.45</v>
+        <v>0.425</v>
       </c>
       <c r="AA36">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AB36">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -3614,7 +3614,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6864629</v>
+        <v>6865299</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
@@ -3623,58 +3623,58 @@
         <v>45186.61458333334</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
         <v>1</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
       </c>
       <c r="I37" t="s">
         <v>42</v>
       </c>
       <c r="J37">
-        <v>1.363</v>
+        <v>1.25</v>
       </c>
       <c r="K37">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="L37">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="M37">
-        <v>1.363</v>
+        <v>1.4</v>
       </c>
       <c r="N37">
-        <v>4.2</v>
+        <v>4.75</v>
       </c>
       <c r="O37">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="P37">
         <v>-1.25</v>
       </c>
       <c r="Q37">
+        <v>1.9</v>
+      </c>
+      <c r="R37">
+        <v>1.9</v>
+      </c>
+      <c r="S37">
+        <v>2.75</v>
+      </c>
+      <c r="T37">
+        <v>1.85</v>
+      </c>
+      <c r="U37">
         <v>1.95</v>
       </c>
-      <c r="R37">
-        <v>1.85</v>
-      </c>
-      <c r="S37">
-        <v>2.5</v>
-      </c>
-      <c r="T37">
-        <v>1.925</v>
-      </c>
-      <c r="U37">
-        <v>1.875</v>
-      </c>
       <c r="V37">
-        <v>0.363</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W37">
         <v>-1</v>
@@ -3686,13 +3686,13 @@
         <v>-0.5</v>
       </c>
       <c r="Z37">
+        <v>0.45</v>
+      </c>
+      <c r="AA37">
         <v>0.425</v>
       </c>
-      <c r="AA37">
-        <v>-1</v>
-      </c>
       <c r="AB37">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -4646,7 +4646,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6865310</v>
+        <v>6865311</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -4655,76 +4655,76 @@
         <v>45200.41666666666</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F49" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H49">
         <v>2</v>
       </c>
       <c r="I49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J49">
-        <v>3.4</v>
+        <v>1.833</v>
       </c>
       <c r="K49">
         <v>3.6</v>
       </c>
       <c r="L49">
-        <v>1.833</v>
+        <v>3.4</v>
       </c>
       <c r="M49">
-        <v>4.75</v>
+        <v>1.909</v>
       </c>
       <c r="N49">
-        <v>4.75</v>
+        <v>3.4</v>
       </c>
       <c r="O49">
-        <v>1.45</v>
+        <v>3.3</v>
       </c>
       <c r="P49">
-        <v>1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q49">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="R49">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="S49">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T49">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U49">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V49">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="W49">
         <v>-1</v>
       </c>
       <c r="X49">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="Y49">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z49">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA49">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB49">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="50" spans="1:28">
@@ -4732,7 +4732,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>6865311</v>
+        <v>6865310</v>
       </c>
       <c r="C50" t="s">
         <v>27</v>
@@ -4741,76 +4741,76 @@
         <v>45200.41666666666</v>
       </c>
       <c r="E50" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F50" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J50">
-        <v>1.833</v>
+        <v>3.4</v>
       </c>
       <c r="K50">
         <v>3.6</v>
       </c>
       <c r="L50">
-        <v>3.4</v>
+        <v>1.833</v>
       </c>
       <c r="M50">
-        <v>1.909</v>
+        <v>4.75</v>
       </c>
       <c r="N50">
-        <v>3.4</v>
+        <v>4.75</v>
       </c>
       <c r="O50">
-        <v>3.3</v>
+        <v>1.45</v>
       </c>
       <c r="P50">
-        <v>-0.5</v>
+        <v>1.25</v>
       </c>
       <c r="Q50">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="R50">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S50">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T50">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="U50">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V50">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="W50">
         <v>-1</v>
       </c>
       <c r="X50">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Y50">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="Z50">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA50">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB50">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="51" spans="1:28">
@@ -6968,7 +6968,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>6865377</v>
+        <v>6865328</v>
       </c>
       <c r="C76" t="s">
         <v>27</v>
@@ -6977,76 +6977,76 @@
         <v>45235.375</v>
       </c>
       <c r="E76" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F76" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J76">
-        <v>1.333</v>
+        <v>2</v>
       </c>
       <c r="K76">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L76">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M76">
-        <v>1.166</v>
+        <v>2.1</v>
       </c>
       <c r="N76">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="O76">
-        <v>13</v>
+        <v>3.3</v>
       </c>
       <c r="P76">
-        <v>-2</v>
+        <v>-0.25</v>
       </c>
       <c r="Q76">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="R76">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S76">
-        <v>3.25</v>
+        <v>2</v>
       </c>
       <c r="T76">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="U76">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V76">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W76">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X76">
         <v>-1</v>
       </c>
       <c r="Y76">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Z76">
-        <v>0</v>
+        <v>0.4875</v>
       </c>
       <c r="AA76">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AB76">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:28">
@@ -7054,7 +7054,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>6865328</v>
+        <v>6865377</v>
       </c>
       <c r="C77" t="s">
         <v>27</v>
@@ -7063,76 +7063,76 @@
         <v>45235.375</v>
       </c>
       <c r="E77" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F77" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J77">
-        <v>2</v>
+        <v>1.333</v>
       </c>
       <c r="K77">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L77">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M77">
-        <v>2.1</v>
+        <v>1.166</v>
       </c>
       <c r="N77">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="O77">
-        <v>3.3</v>
+        <v>13</v>
       </c>
       <c r="P77">
-        <v>-0.25</v>
+        <v>-2</v>
       </c>
       <c r="Q77">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="R77">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S77">
-        <v>2</v>
+        <v>3.25</v>
       </c>
       <c r="T77">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U77">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V77">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="W77">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X77">
         <v>-1</v>
       </c>
       <c r="Y77">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Z77">
-        <v>0.4875</v>
+        <v>0</v>
       </c>
       <c r="AA77">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AB77">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="78" spans="1:28">
@@ -7914,7 +7914,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>7505495</v>
+        <v>7505497</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
@@ -7923,76 +7923,76 @@
         <v>45256.375</v>
       </c>
       <c r="E87" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F87" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J87">
-        <v>1.444</v>
+        <v>1.65</v>
       </c>
       <c r="K87">
+        <v>3.4</v>
+      </c>
+      <c r="L87">
+        <v>4.75</v>
+      </c>
+      <c r="M87">
+        <v>1.8</v>
+      </c>
+      <c r="N87">
+        <v>3.2</v>
+      </c>
+      <c r="O87">
         <v>4.2</v>
       </c>
-      <c r="L87">
-        <v>5.5</v>
-      </c>
-      <c r="M87">
-        <v>1.5</v>
-      </c>
-      <c r="N87">
-        <v>4.2</v>
-      </c>
-      <c r="O87">
-        <v>5.25</v>
-      </c>
       <c r="P87">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Q87">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="R87">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="S87">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="T87">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="U87">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="V87">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="W87">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="X87">
         <v>-1</v>
       </c>
       <c r="Y87">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z87">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA87">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB87">
-        <v>1.025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:28">
@@ -8000,7 +8000,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>7505497</v>
+        <v>7505495</v>
       </c>
       <c r="C88" t="s">
         <v>27</v>
@@ -8009,76 +8009,76 @@
         <v>45256.375</v>
       </c>
       <c r="E88" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F88" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G88">
         <v>1</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J88">
-        <v>1.65</v>
+        <v>1.444</v>
       </c>
       <c r="K88">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="L88">
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="M88">
+        <v>1.5</v>
+      </c>
+      <c r="N88">
+        <v>4.2</v>
+      </c>
+      <c r="O88">
+        <v>5.25</v>
+      </c>
+      <c r="P88">
+        <v>-1</v>
+      </c>
+      <c r="Q88">
         <v>1.8</v>
       </c>
-      <c r="N88">
-        <v>3.2</v>
-      </c>
-      <c r="O88">
-        <v>4.2</v>
-      </c>
-      <c r="P88">
-        <v>-0.5</v>
-      </c>
-      <c r="Q88">
-        <v>1.825</v>
-      </c>
       <c r="R88">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S88">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="T88">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="U88">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="V88">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="W88">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="X88">
         <v>-1</v>
       </c>
       <c r="Y88">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Z88">
-        <v>0.9750000000000001</v>
+        <v>0</v>
       </c>
       <c r="AA88">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB88">
-        <v>0</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="89" spans="1:28">
@@ -9978,7 +9978,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>6865352</v>
+        <v>6865354</v>
       </c>
       <c r="C111" t="s">
         <v>27</v>
@@ -9987,76 +9987,76 @@
         <v>45339.375</v>
       </c>
       <c r="E111" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F111" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H111">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I111" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J111">
-        <v>1.615</v>
+        <v>1.8</v>
       </c>
       <c r="K111">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="L111">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="M111">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="N111">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="O111">
-        <v>5.75</v>
+        <v>2.9</v>
       </c>
       <c r="P111">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q111">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="R111">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="S111">
         <v>2.25</v>
       </c>
       <c r="T111">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="U111">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V111">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="W111">
         <v>-1</v>
       </c>
       <c r="X111">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="Y111">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z111">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA111">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
       <c r="AB111">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="112" spans="1:28">
@@ -10064,7 +10064,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>6865354</v>
+        <v>6865352</v>
       </c>
       <c r="C112" t="s">
         <v>27</v>
@@ -10073,76 +10073,76 @@
         <v>45339.375</v>
       </c>
       <c r="E112" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F112" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J112">
-        <v>1.8</v>
+        <v>1.615</v>
       </c>
       <c r="K112">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="M112">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="N112">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="O112">
-        <v>2.9</v>
+        <v>5.75</v>
       </c>
       <c r="P112">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q112">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="R112">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
         <v>2.25</v>
       </c>
       <c r="T112">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="U112">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V112">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z112">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA112">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
       <c r="AB112">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -15654,7 +15654,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>7952767</v>
+        <v>7952769</v>
       </c>
       <c r="C177" t="s">
         <v>27</v>
@@ -15663,10 +15663,10 @@
         <v>45415.54166666666</v>
       </c>
       <c r="E177" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F177" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G177">
         <v>2</v>
@@ -15678,43 +15678,43 @@
         <v>42</v>
       </c>
       <c r="J177">
-        <v>1.727</v>
+        <v>1.666</v>
       </c>
       <c r="K177">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="L177">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="M177">
-        <v>1.3</v>
+        <v>1.333</v>
       </c>
       <c r="N177">
-        <v>4.333</v>
+        <v>4.2</v>
       </c>
       <c r="O177">
         <v>8</v>
       </c>
       <c r="P177">
-        <v>-1.5</v>
+        <v>-1.25</v>
       </c>
       <c r="Q177">
+        <v>1.85</v>
+      </c>
+      <c r="R177">
         <v>1.95</v>
       </c>
-      <c r="R177">
-        <v>1.85</v>
-      </c>
       <c r="S177">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T177">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="U177">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="V177">
-        <v>0.3</v>
+        <v>0.333</v>
       </c>
       <c r="W177">
         <v>-1</v>
@@ -15723,16 +15723,16 @@
         <v>-1</v>
       </c>
       <c r="Y177">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z177">
         <v>-1</v>
       </c>
       <c r="AA177">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB177">
-        <v>0.95</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="178" spans="1:28">
@@ -15740,7 +15740,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>7952769</v>
+        <v>7952767</v>
       </c>
       <c r="C178" t="s">
         <v>27</v>
@@ -15749,10 +15749,10 @@
         <v>45415.54166666666</v>
       </c>
       <c r="E178" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F178" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G178">
         <v>2</v>
@@ -15764,43 +15764,43 @@
         <v>42</v>
       </c>
       <c r="J178">
-        <v>1.666</v>
+        <v>1.727</v>
       </c>
       <c r="K178">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="L178">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
       <c r="M178">
-        <v>1.333</v>
+        <v>1.3</v>
       </c>
       <c r="N178">
-        <v>4.2</v>
+        <v>4.333</v>
       </c>
       <c r="O178">
         <v>8</v>
       </c>
       <c r="P178">
-        <v>-1.25</v>
+        <v>-1.5</v>
       </c>
       <c r="Q178">
+        <v>1.95</v>
+      </c>
+      <c r="R178">
         <v>1.85</v>
       </c>
-      <c r="R178">
+      <c r="S178">
+        <v>2.75</v>
+      </c>
+      <c r="T178">
+        <v>1.85</v>
+      </c>
+      <c r="U178">
         <v>1.95</v>
       </c>
-      <c r="S178">
-        <v>2.25</v>
-      </c>
-      <c r="T178">
-        <v>1.9</v>
-      </c>
-      <c r="U178">
-        <v>1.9</v>
-      </c>
       <c r="V178">
-        <v>0.333</v>
+        <v>0.3</v>
       </c>
       <c r="W178">
         <v>-1</v>
@@ -15809,16 +15809,16 @@
         <v>-1</v>
       </c>
       <c r="Y178">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="Z178">
         <v>-1</v>
       </c>
       <c r="AA178">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB178">
-        <v>0.45</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="179" spans="1:28">
@@ -16678,6 +16678,522 @@
         <v>0.9750000000000001</v>
       </c>
       <c r="AB188">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:28">
+      <c r="A189" s="1">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>7952781</v>
+      </c>
+      <c r="C189" t="s">
+        <v>27</v>
+      </c>
+      <c r="D189" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E189" t="s">
+        <v>32</v>
+      </c>
+      <c r="F189" t="s">
+        <v>34</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>5</v>
+      </c>
+      <c r="I189" t="s">
+        <v>43</v>
+      </c>
+      <c r="J189">
+        <v>2.15</v>
+      </c>
+      <c r="K189">
+        <v>3.25</v>
+      </c>
+      <c r="L189">
+        <v>2.9</v>
+      </c>
+      <c r="M189">
+        <v>3.6</v>
+      </c>
+      <c r="N189">
+        <v>3.4</v>
+      </c>
+      <c r="O189">
+        <v>1.85</v>
+      </c>
+      <c r="P189">
+        <v>0.5</v>
+      </c>
+      <c r="Q189">
+        <v>1.875</v>
+      </c>
+      <c r="R189">
+        <v>1.925</v>
+      </c>
+      <c r="S189">
+        <v>2.5</v>
+      </c>
+      <c r="T189">
+        <v>1.975</v>
+      </c>
+      <c r="U189">
+        <v>1.825</v>
+      </c>
+      <c r="V189">
+        <v>-1</v>
+      </c>
+      <c r="W189">
+        <v>-1</v>
+      </c>
+      <c r="X189">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="Y189">
+        <v>-1</v>
+      </c>
+      <c r="Z189">
+        <v>0.925</v>
+      </c>
+      <c r="AA189">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB189">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:28">
+      <c r="A190" s="1">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>7952776</v>
+      </c>
+      <c r="C190" t="s">
+        <v>27</v>
+      </c>
+      <c r="D190" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E190" t="s">
+        <v>30</v>
+      </c>
+      <c r="F190" t="s">
+        <v>31</v>
+      </c>
+      <c r="G190">
+        <v>1</v>
+      </c>
+      <c r="H190">
+        <v>1</v>
+      </c>
+      <c r="I190" t="s">
+        <v>44</v>
+      </c>
+      <c r="J190">
+        <v>1.571</v>
+      </c>
+      <c r="K190">
+        <v>3.4</v>
+      </c>
+      <c r="L190">
+        <v>5.5</v>
+      </c>
+      <c r="M190">
+        <v>1.363</v>
+      </c>
+      <c r="N190">
+        <v>3.9</v>
+      </c>
+      <c r="O190">
+        <v>8</v>
+      </c>
+      <c r="P190">
+        <v>-1.25</v>
+      </c>
+      <c r="Q190">
+        <v>1.85</v>
+      </c>
+      <c r="R190">
+        <v>1.95</v>
+      </c>
+      <c r="S190">
+        <v>2.75</v>
+      </c>
+      <c r="T190">
+        <v>1.925</v>
+      </c>
+      <c r="U190">
+        <v>1.875</v>
+      </c>
+      <c r="V190">
+        <v>-1</v>
+      </c>
+      <c r="W190">
+        <v>2.9</v>
+      </c>
+      <c r="X190">
+        <v>-1</v>
+      </c>
+      <c r="Y190">
+        <v>-1</v>
+      </c>
+      <c r="Z190">
+        <v>0.95</v>
+      </c>
+      <c r="AA190">
+        <v>-1</v>
+      </c>
+      <c r="AB190">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="191" spans="1:28">
+      <c r="A191" s="1">
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <v>7952780</v>
+      </c>
+      <c r="C191" t="s">
+        <v>27</v>
+      </c>
+      <c r="D191" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E191" t="s">
+        <v>28</v>
+      </c>
+      <c r="F191" t="s">
+        <v>29</v>
+      </c>
+      <c r="G191">
+        <v>3</v>
+      </c>
+      <c r="H191">
+        <v>3</v>
+      </c>
+      <c r="I191" t="s">
+        <v>44</v>
+      </c>
+      <c r="J191">
+        <v>1.4</v>
+      </c>
+      <c r="K191">
+        <v>4</v>
+      </c>
+      <c r="L191">
+        <v>7</v>
+      </c>
+      <c r="M191">
+        <v>1.363</v>
+      </c>
+      <c r="N191">
+        <v>4.2</v>
+      </c>
+      <c r="O191">
+        <v>8</v>
+      </c>
+      <c r="P191">
+        <v>-1.5</v>
+      </c>
+      <c r="Q191">
+        <v>2</v>
+      </c>
+      <c r="R191">
+        <v>1.8</v>
+      </c>
+      <c r="S191">
+        <v>2.75</v>
+      </c>
+      <c r="T191">
+        <v>1.825</v>
+      </c>
+      <c r="U191">
+        <v>1.975</v>
+      </c>
+      <c r="V191">
+        <v>-1</v>
+      </c>
+      <c r="W191">
+        <v>3.2</v>
+      </c>
+      <c r="X191">
+        <v>-1</v>
+      </c>
+      <c r="Y191">
+        <v>-1</v>
+      </c>
+      <c r="Z191">
+        <v>0.8</v>
+      </c>
+      <c r="AA191">
+        <v>0.825</v>
+      </c>
+      <c r="AB191">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:28">
+      <c r="A192" s="1">
+        <v>190</v>
+      </c>
+      <c r="B192">
+        <v>7952777</v>
+      </c>
+      <c r="C192" t="s">
+        <v>27</v>
+      </c>
+      <c r="D192" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E192" t="s">
+        <v>36</v>
+      </c>
+      <c r="F192" t="s">
+        <v>33</v>
+      </c>
+      <c r="G192">
+        <v>4</v>
+      </c>
+      <c r="H192">
+        <v>3</v>
+      </c>
+      <c r="I192" t="s">
+        <v>42</v>
+      </c>
+      <c r="J192">
+        <v>1.25</v>
+      </c>
+      <c r="K192">
+        <v>5.75</v>
+      </c>
+      <c r="L192">
+        <v>7</v>
+      </c>
+      <c r="M192">
+        <v>1.2</v>
+      </c>
+      <c r="N192">
+        <v>5.75</v>
+      </c>
+      <c r="O192">
+        <v>12</v>
+      </c>
+      <c r="P192">
+        <v>-2</v>
+      </c>
+      <c r="Q192">
+        <v>1.95</v>
+      </c>
+      <c r="R192">
+        <v>1.85</v>
+      </c>
+      <c r="S192">
+        <v>3.25</v>
+      </c>
+      <c r="T192">
+        <v>1.9</v>
+      </c>
+      <c r="U192">
+        <v>1.9</v>
+      </c>
+      <c r="V192">
+        <v>0.2</v>
+      </c>
+      <c r="W192">
+        <v>-1</v>
+      </c>
+      <c r="X192">
+        <v>-1</v>
+      </c>
+      <c r="Y192">
+        <v>-1</v>
+      </c>
+      <c r="Z192">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AA192">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AB192">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:28">
+      <c r="A193" s="1">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>7952779</v>
+      </c>
+      <c r="C193" t="s">
+        <v>27</v>
+      </c>
+      <c r="D193" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E193" t="s">
+        <v>37</v>
+      </c>
+      <c r="F193" t="s">
+        <v>38</v>
+      </c>
+      <c r="G193">
+        <v>4</v>
+      </c>
+      <c r="H193">
+        <v>0</v>
+      </c>
+      <c r="I193" t="s">
+        <v>42</v>
+      </c>
+      <c r="J193">
+        <v>1.25</v>
+      </c>
+      <c r="K193">
+        <v>5.75</v>
+      </c>
+      <c r="L193">
+        <v>7</v>
+      </c>
+      <c r="M193">
+        <v>1.055</v>
+      </c>
+      <c r="N193">
+        <v>13</v>
+      </c>
+      <c r="O193">
+        <v>17</v>
+      </c>
+      <c r="P193">
+        <v>-3.5</v>
+      </c>
+      <c r="Q193">
+        <v>1.975</v>
+      </c>
+      <c r="R193">
+        <v>1.825</v>
+      </c>
+      <c r="S193">
+        <v>4.75</v>
+      </c>
+      <c r="T193">
+        <v>1.825</v>
+      </c>
+      <c r="U193">
+        <v>1.975</v>
+      </c>
+      <c r="V193">
+        <v>0.05499999999999994</v>
+      </c>
+      <c r="W193">
+        <v>-1</v>
+      </c>
+      <c r="X193">
+        <v>-1</v>
+      </c>
+      <c r="Y193">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="Z193">
+        <v>-1</v>
+      </c>
+      <c r="AA193">
+        <v>-1</v>
+      </c>
+      <c r="AB193">
+        <v>0.9750000000000001</v>
+      </c>
+    </row>
+    <row r="194" spans="1:28">
+      <c r="A194" s="1">
+        <v>192</v>
+      </c>
+      <c r="B194">
+        <v>7952778</v>
+      </c>
+      <c r="C194" t="s">
+        <v>27</v>
+      </c>
+      <c r="D194" s="2">
+        <v>45432.5</v>
+      </c>
+      <c r="E194" t="s">
+        <v>39</v>
+      </c>
+      <c r="F194" t="s">
+        <v>35</v>
+      </c>
+      <c r="G194">
+        <v>2</v>
+      </c>
+      <c r="H194">
+        <v>3</v>
+      </c>
+      <c r="I194" t="s">
+        <v>43</v>
+      </c>
+      <c r="J194">
+        <v>1.727</v>
+      </c>
+      <c r="K194">
+        <v>3.75</v>
+      </c>
+      <c r="L194">
+        <v>3.75</v>
+      </c>
+      <c r="M194">
+        <v>1.7</v>
+      </c>
+      <c r="N194">
+        <v>3.9</v>
+      </c>
+      <c r="O194">
+        <v>3.9</v>
+      </c>
+      <c r="P194">
+        <v>-0.75</v>
+      </c>
+      <c r="Q194">
+        <v>1.975</v>
+      </c>
+      <c r="R194">
+        <v>1.825</v>
+      </c>
+      <c r="S194">
+        <v>2.25</v>
+      </c>
+      <c r="T194">
+        <v>1.8</v>
+      </c>
+      <c r="U194">
+        <v>2</v>
+      </c>
+      <c r="V194">
+        <v>-1</v>
+      </c>
+      <c r="W194">
+        <v>-1</v>
+      </c>
+      <c r="X194">
+        <v>2.9</v>
+      </c>
+      <c r="Y194">
+        <v>-1</v>
+      </c>
+      <c r="Z194">
+        <v>0.825</v>
+      </c>
+      <c r="AA194">
+        <v>0.8</v>
+      </c>
+      <c r="AB194">
         <v>-1</v>
       </c>
     </row>

</xml_diff>